<commit_message>
[joy] : latest backend code
</commit_message>
<xml_diff>
--- a/u2l_backend/report_templates/java_report.xlsx
+++ b/u2l_backend/report_templates/java_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pahari\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pahari\Desktop\Project_updates\Old Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D030CDE6-4890-492C-A2CB-4E03D9E7C9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86354D2C-DDF4-4423-8C2F-49114C55BEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="871" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <sheet name="JDK Anaylsis Details" sheetId="13" r:id="rId8"/>
     <sheet name="Import JSP Report" sheetId="17" r:id="rId9"/>
     <sheet name="Compilation Warning Report" sheetId="15" r:id="rId10"/>
-    <sheet name="javaAffectedSourceInformation" sheetId="19" r:id="rId11"/>
-    <sheet name="javaSourceCode2Remedy" sheetId="20" r:id="rId12"/>
-    <sheet name="javaSourceScanRemedy" sheetId="21" r:id="rId13"/>
+    <sheet name="javaSourceCode2Remedy" sheetId="20" r:id="rId11"/>
+    <sheet name="javaSourceScanRemedy" sheetId="21" r:id="rId12"/>
+    <sheet name="Best_Practices" sheetId="22" r:id="rId13"/>
+    <sheet name="Multithreading" sheetId="23" r:id="rId14"/>
+    <sheet name="Performance" sheetId="25" r:id="rId15"/>
+    <sheet name="Security" sheetId="26" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="153">
   <si>
     <t>Prepared by:</t>
   </si>
@@ -1476,6 +1479,27 @@
   </si>
   <si>
     <t>REMEDY</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Rule set</t>
+  </si>
+  <si>
+    <t>Rule</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1825,31 +1849,19 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1858,7 +1870,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1869,6 +1893,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2161,7 +2188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2203,18 +2230,18 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
       <c r="M7" s="12"/>
     </row>
     <row r="8" spans="2:13" ht="25" x14ac:dyDescent="0.5">
       <c r="B8" s="12"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="G8" s="1"/>
       <c r="M8" s="12"/>
     </row>
@@ -2821,451 +2848,12 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE40A81-A5E8-4FF4-B580-92EC2FD64658}">
-  <dimension ref="A1:F51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB063408-A8DE-465C-8E0F-06AE3ED48FCE}">
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="6.6328125" customWidth="1"/>
-    <col min="2" max="2" width="37.08984375" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.6328125" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="24"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="24"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="24"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="24"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="24"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="24"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="24"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="24"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="24"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB063408-A8DE-465C-8E0F-06AE3ED48FCE}">
-  <dimension ref="A1:G51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3274,11 +2862,12 @@
     <col min="3" max="3" width="51.1796875" customWidth="1"/>
     <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>23</v>
       </c>
@@ -3292,16 +2881,19 @@
         <v>25</v>
       </c>
       <c r="E1" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="24"/>
       <c r="B2" s="26"/>
       <c r="C2" s="25"/>
@@ -3309,8 +2901,9 @@
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="24"/>
       <c r="B3" s="26"/>
       <c r="C3" s="25"/>
@@ -3318,8 +2911,9 @@
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="26"/>
       <c r="C4" s="25"/>
@@ -3327,8 +2921,9 @@
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="26"/>
       <c r="C5" s="25"/>
@@ -3336,8 +2931,9 @@
       <c r="E5" s="26"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="26"/>
       <c r="C6" s="25"/>
@@ -3345,8 +2941,9 @@
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="26"/>
       <c r="C7" s="25"/>
@@ -3354,8 +2951,9 @@
       <c r="E7" s="26"/>
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="26"/>
       <c r="C8" s="25"/>
@@ -3363,8 +2961,9 @@
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="26"/>
       <c r="C9" s="25"/>
@@ -3372,8 +2971,9 @@
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="26"/>
       <c r="C10" s="25"/>
@@ -3381,8 +2981,9 @@
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="26"/>
       <c r="C11" s="25"/>
@@ -3390,8 +2991,9 @@
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="26"/>
       <c r="C12" s="25"/>
@@ -3399,8 +3001,9 @@
       <c r="E12" s="26"/>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="26"/>
       <c r="C13" s="25"/>
@@ -3408,8 +3011,9 @@
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="26"/>
       <c r="C14" s="25"/>
@@ -3417,8 +3021,9 @@
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="26"/>
       <c r="C15" s="25"/>
@@ -3426,8 +3031,9 @@
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="26"/>
       <c r="C16" s="25"/>
@@ -3435,8 +3041,9 @@
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
       <c r="G16" s="26"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
       <c r="B17" s="26"/>
       <c r="C17" s="25"/>
@@ -3444,8 +3051,9 @@
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="24"/>
       <c r="B18" s="26"/>
       <c r="C18" s="25"/>
@@ -3453,8 +3061,9 @@
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
       <c r="G18" s="26"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="24"/>
       <c r="B19" s="26"/>
       <c r="C19" s="25"/>
@@ -3462,8 +3071,9 @@
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="26"/>
       <c r="C20" s="25"/>
@@ -3471,8 +3081,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="26"/>
       <c r="C21" s="25"/>
@@ -3480,8 +3091,9 @@
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="26"/>
       <c r="C22" s="25"/>
@@ -3489,8 +3101,9 @@
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
       <c r="G22" s="26"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="26"/>
       <c r="C23" s="25"/>
@@ -3498,8 +3111,9 @@
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
       <c r="G23" s="26"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="26"/>
       <c r="C24" s="25"/>
@@ -3507,8 +3121,9 @@
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
       <c r="G24" s="26"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" s="26"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="26"/>
       <c r="C25" s="25"/>
@@ -3516,8 +3131,9 @@
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
       <c r="G25" s="26"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" s="26"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="26"/>
       <c r="C26" s="25"/>
@@ -3525,8 +3141,9 @@
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" s="26"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
       <c r="C27" s="25"/>
@@ -3534,8 +3151,9 @@
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
       <c r="G27" s="26"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="24"/>
       <c r="B28" s="26"/>
       <c r="C28" s="25"/>
@@ -3543,8 +3161,9 @@
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
       <c r="G28" s="26"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="24"/>
       <c r="B29" s="26"/>
       <c r="C29" s="25"/>
@@ -3552,8 +3171,9 @@
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="24"/>
       <c r="B30" s="26"/>
       <c r="C30" s="25"/>
@@ -3561,8 +3181,9 @@
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="24"/>
       <c r="B31" s="26"/>
       <c r="C31" s="25"/>
@@ -3570,8 +3191,9 @@
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" s="26"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="24"/>
       <c r="B32" s="26"/>
       <c r="C32" s="25"/>
@@ -3579,8 +3201,9 @@
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" s="26"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="24"/>
       <c r="B33" s="26"/>
       <c r="C33" s="25"/>
@@ -3588,8 +3211,9 @@
       <c r="E33" s="26"/>
       <c r="F33" s="26"/>
       <c r="G33" s="26"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" s="26"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="24"/>
       <c r="B34" s="26"/>
       <c r="C34" s="25"/>
@@ -3597,8 +3221,9 @@
       <c r="E34" s="26"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" s="26"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="24"/>
       <c r="B35" s="26"/>
       <c r="C35" s="25"/>
@@ -3606,8 +3231,9 @@
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" s="26"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="26"/>
       <c r="C36" s="25"/>
@@ -3615,8 +3241,9 @@
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" s="26"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="24"/>
       <c r="B37" s="26"/>
       <c r="C37" s="25"/>
@@ -3624,8 +3251,9 @@
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
       <c r="G37" s="26"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" s="26"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="24"/>
       <c r="B38" s="26"/>
       <c r="C38" s="25"/>
@@ -3633,8 +3261,9 @@
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" s="26"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="24"/>
       <c r="B39" s="26"/>
       <c r="C39" s="25"/>
@@ -3642,8 +3271,9 @@
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" s="26"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="24"/>
       <c r="B40" s="26"/>
       <c r="C40" s="25"/>
@@ -3651,8 +3281,9 @@
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="24"/>
       <c r="B41" s="26"/>
       <c r="C41" s="25"/>
@@ -3660,8 +3291,9 @@
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" s="26"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="24"/>
       <c r="B42" s="26"/>
       <c r="C42" s="25"/>
@@ -3669,8 +3301,9 @@
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" s="26"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
       <c r="B43" s="26"/>
       <c r="C43" s="25"/>
@@ -3678,8 +3311,9 @@
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
       <c r="G43" s="26"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" s="26"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="24"/>
       <c r="B44" s="26"/>
       <c r="C44" s="25"/>
@@ -3687,8 +3321,9 @@
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" s="26"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="24"/>
       <c r="B45" s="26"/>
       <c r="C45" s="25"/>
@@ -3696,8 +3331,9 @@
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="24"/>
       <c r="B46" s="26"/>
       <c r="C46" s="25"/>
@@ -3705,8 +3341,9 @@
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
       <c r="G46" s="26"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46" s="26"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
       <c r="B47" s="26"/>
       <c r="C47" s="25"/>
@@ -3714,8 +3351,9 @@
       <c r="E47" s="26"/>
       <c r="F47" s="26"/>
       <c r="G47" s="26"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H47" s="26"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="24"/>
       <c r="B48" s="26"/>
       <c r="C48" s="25"/>
@@ -3723,8 +3361,9 @@
       <c r="E48" s="26"/>
       <c r="F48" s="26"/>
       <c r="G48" s="26"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48" s="26"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="24"/>
       <c r="B49" s="26"/>
       <c r="C49" s="25"/>
@@ -3732,8 +3371,9 @@
       <c r="E49" s="26"/>
       <c r="F49" s="26"/>
       <c r="G49" s="26"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49" s="26"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="24"/>
       <c r="B50" s="26"/>
       <c r="C50" s="25"/>
@@ -3741,8 +3381,9 @@
       <c r="E50" s="26"/>
       <c r="F50" s="26"/>
       <c r="G50" s="26"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H50" s="26"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="24"/>
       <c r="B51" s="26"/>
       <c r="C51" s="25"/>
@@ -3750,13 +3391,14 @@
       <c r="E51" s="26"/>
       <c r="F51" s="26"/>
       <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154B5582-5ED2-4406-A8C0-7F75CB1116AB}">
   <dimension ref="A1:G51"/>
   <sheetViews>
@@ -4245,6 +3887,218 @@
       <c r="E51" s="26"/>
       <c r="F51" s="26"/>
       <c r="G51" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE20A90-F239-44A7-88BA-E5400EFF05CD}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.08984375" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="32.08984375" customWidth="1"/>
+    <col min="4" max="4" width="39.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.36328125" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C795A117-C679-4DFD-A81E-F8B11C01A880}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.08984375" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="32.08984375" customWidth="1"/>
+    <col min="4" max="4" width="39.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.36328125" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE963A0-5AE0-4708-A3E8-9C0C55635996}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.08984375" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="32.08984375" customWidth="1"/>
+    <col min="4" max="4" width="39.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.36328125" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90AA7DC-CBC8-4BF3-8CAB-65EFBFFD1C24}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.08984375" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="32.08984375" customWidth="1"/>
+    <col min="4" max="4" width="39.7265625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.1796875" customWidth="1"/>
+    <col min="8" max="8" width="28.36328125" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4276,99 +4130,99 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="14" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32" t="s">
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
     </row>
     <row r="13" spans="2:14" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
@@ -4376,232 +4230,232 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="14" x14ac:dyDescent="0.3">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32" t="s">
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32" t="s">
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32" t="s">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32" t="s">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32" t="s">
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32" t="s">
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32" t="s">
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32" t="s">
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32" t="s">
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32" t="s">
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32" t="s">
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
     </row>
     <row r="28" spans="2:14" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B28" s="7" t="s">
@@ -4609,42 +4463,42 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="14" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33" t="s">
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32" t="s">
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
@@ -4653,6 +4507,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:N10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:N16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:N18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:N19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:N20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:N21"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="F30:N30"/>
     <mergeCell ref="B31:E31"/>
@@ -4669,28 +4545,6 @@
     <mergeCell ref="F23:N23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:N24"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:N19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:N20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:N21"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:N16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:N17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:N18"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:N10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:N11"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:N7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:N9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8:E8" location="'Doc Info'!A1" display="Doc Info" xr:uid="{55480A71-F288-48A4-B597-5700C931DEF0}"/>
@@ -4737,58 +4591,58 @@
       </c>
     </row>
     <row r="4" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="34" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="2:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="32"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="2:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="32"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="11" spans="2:10" ht="20" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
@@ -4808,18 +4662,18 @@
       <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="35"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="16"/>
       <c r="F14" s="42"/>
       <c r="G14" s="43"/>
@@ -4894,235 +4748,235 @@
     </row>
     <row r="25" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="19"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40"/>
-      <c r="T25" s="40"/>
-      <c r="U25" s="40"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="36"/>
     </row>
     <row r="26" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="40"/>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40"/>
-      <c r="T26" s="40"/>
-      <c r="U26" s="40"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="36"/>
     </row>
     <row r="27" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="40"/>
-      <c r="U27" s="40"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="36"/>
     </row>
     <row r="28" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40"/>
-      <c r="T28" s="40"/>
-      <c r="U28" s="40"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="36"/>
+      <c r="U28" s="36"/>
     </row>
     <row r="29" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="40"/>
-      <c r="R29" s="40"/>
-      <c r="S29" s="40"/>
-      <c r="T29" s="40"/>
-      <c r="U29" s="40"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+      <c r="U29" s="36"/>
     </row>
     <row r="30" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="19"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="40"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="40"/>
-      <c r="U30" s="40"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
     </row>
     <row r="31" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40"/>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
-      <c r="T31" s="40"/>
-      <c r="U31" s="40"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
     </row>
     <row r="32" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="19"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="40"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="40"/>
-      <c r="R32" s="40"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="40"/>
-      <c r="U32" s="40"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
     </row>
     <row r="33" spans="2:21" ht="13" x14ac:dyDescent="0.3">
       <c r="B33" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="40"/>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="40"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="40"/>
-      <c r="U33" s="40"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
     </row>
     <row r="34" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B34" s="19"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="40"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="40"/>
-      <c r="U34" s="40"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="36"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
     </row>
     <row r="35" spans="2:21" ht="13" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="L35" s="40"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="40"/>
-      <c r="Q35" s="40"/>
-      <c r="R35" s="40"/>
-      <c r="S35" s="40"/>
-      <c r="T35" s="40"/>
-      <c r="U35" s="40"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="36"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="36"/>
+      <c r="R35" s="36"/>
+      <c r="S35" s="36"/>
+      <c r="T35" s="36"/>
+      <c r="U35" s="36"/>
     </row>
     <row r="36" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
-      <c r="P36" s="40"/>
-      <c r="Q36" s="40"/>
-      <c r="R36" s="40"/>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="40"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="36"/>
     </row>
     <row r="37" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="O37" s="40"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="40"/>
-      <c r="R37" s="40"/>
-      <c r="S37" s="40"/>
-      <c r="T37" s="40"/>
-      <c r="U37" s="40"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="36"/>
+      <c r="O37" s="36"/>
+      <c r="P37" s="36"/>
+      <c r="Q37" s="36"/>
+      <c r="R37" s="36"/>
+      <c r="S37" s="36"/>
+      <c r="T37" s="36"/>
+      <c r="U37" s="36"/>
     </row>
     <row r="38" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="40"/>
-      <c r="S38" s="40"/>
-      <c r="T38" s="40"/>
-      <c r="U38" s="40"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="36"/>
+      <c r="O38" s="36"/>
+      <c r="P38" s="36"/>
+      <c r="Q38" s="36"/>
+      <c r="R38" s="36"/>
+      <c r="S38" s="36"/>
+      <c r="T38" s="36"/>
+      <c r="U38" s="36"/>
     </row>
     <row r="39" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
-      <c r="R39" s="40"/>
-      <c r="S39" s="40"/>
-      <c r="T39" s="40"/>
-      <c r="U39" s="40"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="36"/>
+      <c r="S39" s="36"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="36"/>
     </row>
     <row r="40" spans="2:21" ht="13" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="40"/>
-      <c r="S40" s="40"/>
-      <c r="T40" s="40"/>
-      <c r="U40" s="40"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="36"/>
+      <c r="T40" s="36"/>
+      <c r="U40" s="36"/>
     </row>
     <row r="41" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
@@ -5454,6 +5308,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="L25:U40"/>
     <mergeCell ref="F13:J13"/>
     <mergeCell ref="C14:D14"/>
@@ -5469,13 +5330,6 @@
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="F18:J18"/>
     <mergeCell ref="F19:J19"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[joy] : AI driven services integrated
</commit_message>
<xml_diff>
--- a/u2l_backend/report_templates/java_report.xlsx
+++ b/u2l_backend/report_templates/java_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pahari\Desktop\Project_updates\Test n Delete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanip\Documents\test n delete\check\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF35F34-5340-4D9E-B53C-1070E6EB6DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C416C776-FF4F-4074-8D70-EAEBC77F3466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="871" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -1877,34 +1877,37 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1915,9 +1918,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2210,7 +2210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6187,99 +6187,99 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="14" x14ac:dyDescent="0.3">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
     </row>
     <row r="13" spans="2:14" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B13" s="7" t="s">
@@ -6287,232 +6287,232 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="14" x14ac:dyDescent="0.3">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="34" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34" t="s">
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34" t="s">
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
     </row>
     <row r="28" spans="2:14" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B28" s="7" t="s">
@@ -6520,42 +6520,42 @@
       </c>
     </row>
     <row r="30" spans="2:14" ht="14" x14ac:dyDescent="0.3">
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32" t="s">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
@@ -6564,28 +6564,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:N10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:N11"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:N7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:N16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:N17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:N18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:N19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:N20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:N21"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="F30:N30"/>
     <mergeCell ref="B31:E31"/>
@@ -6602,6 +6580,28 @@
     <mergeCell ref="F23:N23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="F24:N24"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:N19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:N20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:N21"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:N16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:N18"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:N10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:N9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8:E8" location="'Doc Info'!A1" display="Doc Info" xr:uid="{55480A71-F288-48A4-B597-5700C931DEF0}"/>
@@ -6701,58 +6701,58 @@
       </c>
     </row>
     <row r="4" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="37" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" spans="2:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="34"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="2:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="2:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="34"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39"/>
     </row>
     <row r="11" spans="2:10" ht="20" x14ac:dyDescent="0.4">
       <c r="B11" s="5" t="s">
@@ -6772,79 +6772,79 @@
       <c r="E13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="36"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="10"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="45"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="44"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="45"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="44"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="45"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="44"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="45"/>
     </row>
     <row r="19" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="44"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="45"/>
     </row>
     <row r="22" spans="2:21" ht="20" x14ac:dyDescent="0.4">
       <c r="B22" s="5" t="s">
@@ -6858,235 +6858,235 @@
     </row>
     <row r="25" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="19"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="36"/>
-      <c r="U25" s="36"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="41"/>
     </row>
     <row r="26" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="36"/>
-      <c r="U26" s="36"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+      <c r="T26" s="41"/>
+      <c r="U26" s="41"/>
     </row>
     <row r="27" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="36"/>
-      <c r="U27" s="36"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
     </row>
     <row r="28" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="41"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+      <c r="T28" s="41"/>
+      <c r="U28" s="41"/>
     </row>
     <row r="29" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="36"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36"/>
-      <c r="U29" s="36"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
     </row>
     <row r="30" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="19"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-      <c r="O30" s="36"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="T30" s="36"/>
-      <c r="U30" s="36"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+      <c r="T30" s="41"/>
+      <c r="U30" s="41"/>
     </row>
     <row r="31" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
     </row>
     <row r="32" spans="2:21" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="19"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+      <c r="T32" s="41"/>
+      <c r="U32" s="41"/>
     </row>
     <row r="33" spans="2:21" ht="13" x14ac:dyDescent="0.3">
       <c r="B33" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="T33" s="36"/>
-      <c r="U33" s="36"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="41"/>
     </row>
     <row r="34" spans="2:21" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B34" s="19"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="36"/>
-      <c r="U34" s="36"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="41"/>
     </row>
     <row r="35" spans="2:21" ht="13" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="36"/>
-      <c r="P35" s="36"/>
-      <c r="Q35" s="36"/>
-      <c r="R35" s="36"/>
-      <c r="S35" s="36"/>
-      <c r="T35" s="36"/>
-      <c r="U35" s="36"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+      <c r="T35" s="41"/>
+      <c r="U35" s="41"/>
     </row>
     <row r="36" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B36" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="36"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="T36" s="36"/>
-      <c r="U36" s="36"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="41"/>
+      <c r="R36" s="41"/>
+      <c r="S36" s="41"/>
+      <c r="T36" s="41"/>
+      <c r="U36" s="41"/>
     </row>
     <row r="37" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="36"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="41"/>
+      <c r="R37" s="41"/>
+      <c r="S37" s="41"/>
+      <c r="T37" s="41"/>
+      <c r="U37" s="41"/>
     </row>
     <row r="38" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="36"/>
-      <c r="T38" s="36"/>
-      <c r="U38" s="36"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+      <c r="O38" s="41"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="41"/>
+      <c r="T38" s="41"/>
+      <c r="U38" s="41"/>
     </row>
     <row r="39" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
+      <c r="P39" s="41"/>
+      <c r="Q39" s="41"/>
+      <c r="R39" s="41"/>
+      <c r="S39" s="41"/>
+      <c r="T39" s="41"/>
+      <c r="U39" s="41"/>
     </row>
     <row r="40" spans="2:21" ht="13" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="T40" s="36"/>
-      <c r="U40" s="36"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="41"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="41"/>
+      <c r="R40" s="41"/>
+      <c r="S40" s="41"/>
+      <c r="T40" s="41"/>
+      <c r="U40" s="41"/>
     </row>
     <row r="41" spans="2:21" ht="13" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
@@ -7418,13 +7418,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="L25:U40"/>
     <mergeCell ref="F13:J13"/>
     <mergeCell ref="C14:D14"/>
@@ -7440,6 +7433,13 @@
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="F18:J18"/>
     <mergeCell ref="F19:J19"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9926,7 +9926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9E1F65-7E82-4C5C-831F-A385EFA6E72F}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>